<commit_message>
Improvements to Admin.xlsx file io
* enabled save of Admin details to xlsx and linked to Confirm Settings button
* forced save of scheme before any weighings are started
* creates folder if folder doesn't exist
* looks for config file in folder and prompts for selection/confirmation if it finds one
* parsing of weight groups now doesn't rely on an Excel formula (which had to be evaluated by Excel for the number to exist)
* updated tests and sample configs to handle these changes
</commit_message>
<xml_diff>
--- a/examples/Admin.xlsx
+++ b/examples/Admin.xlsx
@@ -8,168 +8,181 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578C38F6-7243-4684-810E-B223080AD1BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F978D12-73E5-4003-A4F9-21556B252522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F7F7C31D-9B21-4E63-BF52-B7D512313953}"/>
+    <workbookView xWindow="-28320" yWindow="2910" windowWidth="20640" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="Scheme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>e.g, Set of Weights for Client</t>
+  </si>
+  <si>
+    <t>Subtitle</t>
+  </si>
+  <si>
+    <t>e.g, Weight ID's: X, Y and Z</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Date Opened</t>
+  </si>
   <si>
     <t>Client</t>
   </si>
   <si>
+    <t>The name of the client. Spaces will be removed. Files will be created with this name inside the save folder.</t>
+  </si>
+  <si>
+    <t>Client full address</t>
+  </si>
+  <si>
+    <t>Job Number</t>
+  </si>
+  <si>
+    <t>J00000</t>
+  </si>
+  <si>
+    <t>The J-number job code for the calibration</t>
+  </si>
+  <si>
+    <t>Project Number</t>
+  </si>
+  <si>
+    <t>96240….</t>
+  </si>
+  <si>
+    <t>Save folder</t>
+  </si>
+  <si>
+    <t>The folder in which all data and analysis files are saved</t>
+  </si>
+  <si>
+    <t>Report Number</t>
+  </si>
+  <si>
+    <t>Mass/2021/0000</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Drift correction</t>
+  </si>
+  <si>
+    <t>auto select</t>
+  </si>
+  <si>
+    <t>Specify a drift option to use in the least squares analysis of each circular weighing. Allowed options: auto select, linear drift, quadratic drift, cubic drift</t>
+  </si>
+  <si>
+    <t>Identification</t>
+  </si>
+  <si>
+    <t>Use times?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>&lt;!-- Specify whether to use the recorded times for each mass measurement in the least squares analysis of each circular weighing. Allowed options: YES or NO --&gt;</t>
+  </si>
+  <si>
+    <t>Standards</t>
+  </si>
+  <si>
+    <t>Correlations</t>
+  </si>
+  <si>
+    <t>If relevant, include a matrix/list of correlations between standards (e.g. in build-up or build-down). Allowed options: None, or matrix of correlations</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>MET19A</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>MET19B</t>
+  </si>
+  <si>
+    <t>The reference set used as checks in the weighing scheme. Use tags of sets as in the config.xml file, or None</t>
+  </si>
+  <si>
+    <t>C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\sample_config.xml</t>
+  </si>
+  <si>
+    <t>path to config.xml file containing equipment parameters</t>
+  </si>
+  <si>
     <t>Client weights</t>
   </si>
   <si>
-    <t>Drift correction</t>
-  </si>
-  <si>
-    <t>Save folder</t>
-  </si>
-  <si>
-    <t>Standards</t>
-  </si>
-  <si>
-    <t>MET19B</t>
-  </si>
-  <si>
-    <t>auto select</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Correlations</t>
-  </si>
-  <si>
-    <t>Use times?</t>
-  </si>
-  <si>
-    <t>Specify a drift option to use in the least squares analysis of each circular weighing. Allowed options: auto select, linear drift, quadratic drift, cubic drift</t>
-  </si>
-  <si>
-    <t>&lt;!-- Specify whether to use the recorded times for each mass measurement in the least squares analysis of each circular weighing. Allowed options: YES or NO --&gt;</t>
-  </si>
-  <si>
-    <t>If relevant, include a matrix/list of correlations between standards (e.g. in build-up or build-down). Allowed options: None, or matrix of correlations</t>
+    <t>&lt; can put link to history file here if desired &gt;</t>
+  </si>
+  <si>
+    <t>weight ID</t>
+  </si>
+  <si>
+    <t>Nominal mass /g</t>
+  </si>
+  <si>
+    <t>Distinguishing mark, form or identification*</t>
+  </si>
+  <si>
+    <t>Container ID</t>
+  </si>
+  <si>
+    <t>u_mag /ug</t>
   </si>
   <si>
     <t>Density</t>
   </si>
   <si>
-    <t>96240….</t>
-  </si>
-  <si>
-    <t>Report Number</t>
-  </si>
-  <si>
-    <t>Mass/2021/0000</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Identification</t>
-  </si>
-  <si>
-    <t>Client full address</t>
-  </si>
-  <si>
-    <t>Nominal mass /g</t>
-  </si>
-  <si>
-    <t>Container ID</t>
-  </si>
-  <si>
-    <t>Operator</t>
-  </si>
-  <si>
-    <t>Greg</t>
-  </si>
-  <si>
-    <t>Distinguishing mark, form or identification*</t>
+    <t>u_density</t>
   </si>
   <si>
     <t>* e.g. the symbol or diagram that would usually go in the report</t>
   </si>
   <si>
-    <t>Date Opened</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Check</t>
-  </si>
-  <si>
-    <t>&lt; can put link to history file here if desired &gt;</t>
-  </si>
-  <si>
-    <t>Project Number</t>
-  </si>
-  <si>
-    <t>Job Number</t>
-  </si>
-  <si>
-    <t>Number of weights</t>
-  </si>
-  <si>
-    <t>e.g, Set of Weights for Client</t>
-  </si>
-  <si>
-    <t>u_mag /ug</t>
-  </si>
-  <si>
-    <t>u_density</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
-    <t>Plastic box</t>
+    <t>X</t>
   </si>
   <si>
     <t>200a</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>200b</t>
   </si>
   <si>
     <t>..</t>
   </si>
   <si>
-    <t>ADW</t>
-  </si>
-  <si>
-    <t>CNG</t>
-  </si>
-  <si>
-    <t>weight ID</t>
+    <t>Z</t>
   </si>
   <si>
     <t>Weight groups</t>
@@ -212,27 +225,6 @@
   </si>
   <si>
     <t>5000</t>
-  </si>
-  <si>
-    <t>path to config.xml file containing equipment parameters</t>
-  </si>
-  <si>
-    <t>(calculated automatically)</t>
-  </si>
-  <si>
-    <t>The folder in which all data and analysis files are saved</t>
-  </si>
-  <si>
-    <t>The reference set used as checks in the weighing scheme. Use tags of sets as in the config.xml file, or None</t>
-  </si>
-  <si>
-    <t>The name of the client. Spaces will be removed. Files will be created with this name inside the save folder.</t>
-  </si>
-  <si>
-    <t>The J-number job code for the calibration</t>
-  </si>
-  <si>
-    <t>MET19A</t>
   </si>
 </sst>
 </file>
@@ -314,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -326,27 +318,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -364,24 +347,40 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,18 +694,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AB355D-84BE-43AB-B2BC-CDE069094A48}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6328125" customWidth="1"/>
-    <col min="3" max="3" width="41.81640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="41.81640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18.1796875" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
@@ -715,595 +714,597 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11"/>
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+        <v>9</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" s="3" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>22</v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
+      <c r="A9" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="21" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="17" t="s">
-        <v>59</v>
+        <v>33</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="19"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>30</v>
+      <c r="A13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="24"/>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13">
-        <f>COUNT(B15:B90)</f>
-        <v>3</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>60</v>
-      </c>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>36</v>
+      <c r="G14" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="H14" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
+      <c r="A15" s="11">
         <v>100</v>
       </c>
       <c r="B15" s="1">
         <v>100</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>37</v>
+      <c r="C15" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
-        <v>39</v>
+      <c r="A16" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="B16" s="1">
         <v>200</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>37</v>
+      <c r="C16" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
-        <v>40</v>
+      <c r="A17" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B17" s="1">
         <v>200</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>41</v>
+      <c r="C17" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="14"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="7"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="7"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="7"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="7"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="7"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="18"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="7"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="7"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="7"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="7"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="7"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="7"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="14"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="7"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="14"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="7"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="7"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="7"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="14"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="7"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="14"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="7"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="14"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="7"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="14"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="7"/>
+      <c r="C39" s="18"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="14"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="7"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="14"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="7"/>
+      <c r="C41" s="18"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="14"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="7"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="14"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="7"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="14"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="14"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="7"/>
+      <c r="C45" s="18"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="14"/>
+      <c r="A46" s="11"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="7"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="7"/>
+      <c r="C47" s="18"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="14"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="7"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="14"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="7"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="14"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="7"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="14"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="7"/>
+      <c r="C51" s="18"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="14"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="7"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="14"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="7"/>
+      <c r="C53" s="18"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="14"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="7"/>
+      <c r="C54" s="18"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A55" s="14"/>
+      <c r="A55" s="11"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="7"/>
+      <c r="C55" s="18"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
@@ -1313,22 +1314,23 @@
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{A690A39A-7C4C-498C-8F5B-DEF5027274EF}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"auto select, linear drift, quadratic drift, cubic drift"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{7969CC89-9911-42F9-96DF-8D0F0744D590}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"NO, YES"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDACBCF-9B45-48A5-929B-E05C62DCE908}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1343,60 +1345,60 @@
     <col min="4" max="4" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>48</v>
+    <row r="1" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed example config to default_config.xml
</commit_message>
<xml_diff>
--- a/examples/Admin.xlsx
+++ b/examples/Admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F978D12-73E5-4003-A4F9-21556B252522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCCB0D9-260F-43A4-8B46-1551E176EC86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28320" yWindow="2910" windowWidth="20640" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,6 @@
     <t>The reference set used as checks in the weighing scheme. Use tags of sets as in the config.xml file, or None</t>
   </si>
   <si>
-    <t>C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\sample_config.xml</t>
-  </si>
-  <si>
     <t>path to config.xml file containing equipment parameters</t>
   </si>
   <si>
@@ -225,6 +222,9 @@
   </si>
   <si>
     <t>5000</t>
+  </si>
+  <si>
+    <t>C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\default_config.xml</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -863,11 +863,11 @@
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="28" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -876,38 +876,38 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>38</v>
       </c>
       <c r="C13" s="24"/>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="H14" t="s">
         <v>45</v>
-      </c>
-      <c r="H14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -918,10 +918,10 @@
         <v>100</v>
       </c>
       <c r="C15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -929,16 +929,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1">
         <v>200</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -946,16 +946,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1">
         <v>200</v>
       </c>
       <c r="C17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1347,58 +1347,58 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
       <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
         <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed initial loading of example admin.xlsx file on show_gui
and removed reference to default config file in the example admin.xlsx file
</commit_message>
<xml_diff>
--- a/examples/Admin.xlsx
+++ b/examples/Admin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCCB0D9-260F-43A4-8B46-1551E176EC86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2DCEE6-FFF4-4757-A2DB-AB4529E5EC1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25395" yWindow="1920" windowWidth="20070" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t>Title</t>
   </si>
@@ -206,25 +206,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>1000 1KMA 1KMB</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>AX10005</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>5000 5KMA 5KMB</t>
-  </si>
-  <si>
-    <t>5000</t>
-  </si>
-  <si>
-    <t>C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\default_config.xml</t>
+    <t>Config file</t>
   </si>
 </sst>
 </file>
@@ -697,9 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -861,10 +841,10 @@
       <c r="C11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="28" t="s">
-        <v>67</v>
-      </c>
+      <c r="D11" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="28"/>
       <c r="F11" s="29"/>
       <c r="G11" s="14" t="s">
         <v>35</v>
@@ -1331,11 +1311,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1373,34 +1351,6 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MAJOR COMMIT: reference mass values now come from MassRef.xlsx
* Removed standard set tags from default_config.xml
* Changed parsing of reference mass sets, and some of the dictionary keys for all mass sets.
* Upgraded FinalMassCalc to take dictionary rather than list for client wts
* Upgraded filtering of IDs/mass sets to work for any mass set type.
* Moved some property definitions from Configuration to AdminDetails
* Updated tests to reflect these changes
</commit_message>
<xml_diff>
--- a/examples/Admin.xlsx
+++ b/examples/Admin.xlsx
@@ -8,20 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2DCEE6-FFF4-4757-A2DB-AB4529E5EC1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D917F3-113A-45D4-A9B9-331B250EE152}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25395" yWindow="1920" windowWidth="20070" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="Scheme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Title</t>
   </si>
@@ -104,9 +115,6 @@
     <t>&lt;!-- Specify whether to use the recorded times for each mass measurement in the least squares analysis of each circular weighing. Allowed options: YES or NO --&gt;</t>
   </si>
   <si>
-    <t>Standards</t>
-  </si>
-  <si>
     <t>Correlations</t>
   </si>
   <si>
@@ -116,15 +124,9 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>MET19A</t>
-  </si>
-  <si>
     <t>Check</t>
   </si>
   <si>
-    <t>MET19B</t>
-  </si>
-  <si>
     <t>The reference set used as checks in the weighing scheme. Use tags of sets as in the config.xml file, or None</t>
   </si>
   <si>
@@ -155,9 +157,6 @@
     <t>Density</t>
   </si>
   <si>
-    <t>u_density</t>
-  </si>
-  <si>
     <t>* e.g. the symbol or diagram that would usually go in the report</t>
   </si>
   <si>
@@ -207,6 +206,24 @@
   </si>
   <si>
     <t>Config file</t>
+  </si>
+  <si>
+    <t>Standards file</t>
+  </si>
+  <si>
+    <t>Path to xlsx of standard masses</t>
+  </si>
+  <si>
+    <t>G:\Shared drives\MSL - MAP\mass_setfiles\MASSREF19_4MCW.xlsx</t>
+  </si>
+  <si>
+    <t>Mettler A</t>
+  </si>
+  <si>
+    <t>Mettler B</t>
+  </si>
+  <si>
+    <t>u_dens</t>
   </si>
 </sst>
 </file>
@@ -288,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -334,6 +351,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -679,7 +699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -697,17 +719,17 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="25"/>
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -734,9 +756,9 @@
       <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
@@ -775,79 +797,84 @@
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="21"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -856,38 +883,38 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="24"/>
+        <v>33</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="25"/>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="G14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" t="s">
         <v>41</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -898,10 +925,10 @@
         <v>100</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -909,16 +936,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1">
         <v>200</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -926,16 +953,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1">
         <v>200</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1325,30 +1352,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>